<commit_message>
A working version except the Foliage and NPP dept
</commit_message>
<xml_diff>
--- a/dev/input_data/input_shitai3.xlsx
+++ b/dev/input_data/input_shitai3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81CB609-7EE6-F74F-8267-4A897A2ABC98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3E493-87D6-1C4B-8F7A-83FB123E0DDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
+    <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="2" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1474,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003E9A71-E1A2-2845-B4A9-990606FB2D91}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3763,8 +3763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACAC9B12-40B2-9A4C-94F4-5F3D5BCCC889}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>